<commit_message>
Add Skills On Profile page
</commit_message>
<xml_diff>
--- a/MarsQA-1/SpecflowTests/Data/Mars.xlsx
+++ b/MarsQA-1/SpecflowTests/Data/Mars.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23546d0de25dfd14/Documents/Mars/OnBoarding Task/Advance Task/Mars/MarsQA-1/SpecflowTests/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="11_3E3AA520263A89AAFA20C4EC4F2A22DB7C496A7E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08B0BB16-5FCA-4F0B-BE87-FDE6DD68AF21}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_3E3AA520263A89AAFA20C4EC4F2A22DB7C496A7E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BFB00A7-B3A7-4AF2-A47A-DC238B107D1F}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="16920" windowHeight="9480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="16920" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
     <sheet name="Profile" sheetId="3" r:id="rId2"/>
-    <sheet name="Sign Up" sheetId="2" r:id="rId3"/>
+    <sheet name="Skills" sheetId="4" r:id="rId3"/>
+    <sheet name="Sign Up" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>username</t>
   </si>
@@ -82,6 +83,12 @@
   </si>
   <si>
     <t>Less than $500 per month</t>
+  </si>
+  <si>
+    <t>SkillName</t>
+  </si>
+  <si>
+    <t>C#</t>
   </si>
 </sst>
 </file>
@@ -394,7 +401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1429,7 +1436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A971EFA-FA4A-4C45-B518-5A4316F51C4C}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1477,6 +1484,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F55D26-94C5-41B5-A402-8538748F3597}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E547A0-5D74-49ED-AE17-E8241EC115BA}">
   <dimension ref="A1:F2"/>
   <sheetViews>

</xml_diff>